<commit_message>
Update Optica BAC-05-Catálogo de recursos.xlsx
</commit_message>
<xml_diff>
--- a/HT-4/Optica BAC-05-Catálogo de recursos.xlsx
+++ b/HT-4/Optica BAC-05-Catálogo de recursos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvill\Dropbox\uniandes\MATI\Notas de clase\Artefactos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/juan/Documents/Universidad/2022-20/arquiemp/repo/arquiemp/HT-4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796F8EBD-3BB8-4D90-9B40-4E6CD1282E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5426BED-14AF-5C40-B9F2-104D107AD8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1665" yWindow="525" windowWidth="17445" windowHeight="14910" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
+    <workbookView xWindow="32180" yWindow="-2520" windowWidth="17440" windowHeight="14920" xr2:uid="{6D2ADF59-F33A-44E3-88FB-8431094B32CC}"/>
   </bookViews>
   <sheets>
     <sheet name="BAC-05" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Nombre</t>
   </si>
@@ -49,6 +49,27 @@
   </si>
   <si>
     <t>Modelo de negocio</t>
+  </si>
+  <si>
+    <t>Monturas</t>
+  </si>
+  <si>
+    <t>Lentes</t>
+  </si>
+  <si>
+    <t>Caja registradora</t>
+  </si>
+  <si>
+    <t>Datáfono</t>
+  </si>
+  <si>
+    <t>Laboratorio</t>
+  </si>
+  <si>
+    <t>Consultorio</t>
+  </si>
+  <si>
+    <t>Sistema informático</t>
   </si>
 </sst>
 </file>
@@ -117,11 +138,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -146,7 +166,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -442,75 +462,99 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4ABDEE2F-9DA5-4F4F-A9BF-B9BEA22ACD0E}">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="7.5" customWidth="1"/>
-    <col min="2" max="2" width="39.375" customWidth="1"/>
+    <col min="2" max="2" width="39.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" s="3" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-      <c r="B7" s="5"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-      <c r="B9" s="5"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
-      <c r="B11" s="5"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
+    <row r="6" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A6" s="4">
+        <v>1</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A7" s="4">
+        <v>2</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A8" s="4">
+        <v>3</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A9" s="4">
+        <v>4</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A10" s="4">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A11" s="4">
+        <v>6</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15" x14ac:dyDescent="0.15">
+      <c r="A12" s="4">
+        <v>7</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>